<commit_message>
Added Multiple single column copyies
</commit_message>
<xml_diff>
--- a/Examples/Data.xlsx
+++ b/Examples/Data.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C70B6870-D67E-4E9D-9D84-1A4F414765FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Data</t>
   </si>
@@ -37,12 +39,48 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,11 +391,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -401,4 +439,105 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0CBE1E-8368-4471-9BCC-A22D4F499364}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix single column range
</commit_message>
<xml_diff>
--- a/Examples/Data.xlsx
+++ b/Examples/Data.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C70B6870-D67E-4E9D-9D84-1A4F414765FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Data</t>
   </si>
@@ -80,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,12 +390,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,98 +441,119 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0CBE1E-8368-4471-9BCC-A22D4F499364}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:A17"/>
+  <dimension ref="D1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="N4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="N5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="N6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="N7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="N9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="N10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>